<commit_message>
fix: update some commits
</commit_message>
<xml_diff>
--- a/src/demo/doc/lc.xlsx
+++ b/src/demo/doc/lc.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eehongzhijun\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hongzhijun\prj\leetcode\src\demo\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEBBD7C-0E4A-494B-A013-1D156F7872A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17481E4-3231-4DC9-BF0E-579DCB5BFBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0E398A26-88E2-441B-977B-61641413524A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{0E398A26-88E2-441B-977B-61641413524A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="231028" sheetId="2" r:id="rId1"/>
+    <sheet name="231027" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>dp[0]</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,6 +68,33 @@
   </si>
   <si>
     <t>max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>91. 解码方法 - 力扣（LeetCode）</t>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/2, 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/2/3, 12/3, 1/23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/2/3/4, 12/3/4, 1/23/4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -125,7 +153,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -143,6 +171,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -241,7 +278,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$N$4</c:f>
+              <c:f>'231027'!$F$4:$N$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1333,11 +1370,242 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130001C2-CB08-43A0-BF93-B7C181D475AC}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="29.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="str">
+        <f>CHAR(64+ROW())</f>
+        <v>A</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f t="shared" ref="A2:A26" si="0">CHAR(64+ROW())</f>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>G</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>H</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>I</v>
+      </c>
+      <c r="B9">
+        <v>123</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>J</v>
+      </c>
+      <c r="B10">
+        <v>1234</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>K</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>O</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>P</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>Q</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>R</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>U</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>V</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>W</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v>Z</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="https://leetcode.cn/problems/decode-ways/" xr:uid="{3C001209-180C-488E-9536-C1E81FCCCB31}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <ignoredErrors>
+    <ignoredError sqref="C8" twoDigitTextYear="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F47A53-2DB9-4A8A-A38A-83432DAA38DE}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>